<commit_message>
freedom to choose side and excercise added
</commit_message>
<xml_diff>
--- a/resultados_dips/resultados_dips.xlsx
+++ b/resultados_dips/resultados_dips.xlsx
@@ -466,7 +466,7 @@
         <v>285.02</v>
       </c>
       <c r="D2" t="n">
-        <v>0.39</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="3">
@@ -480,7 +480,7 @@
         <v>290.45</v>
       </c>
       <c r="D3" t="n">
-        <v>0.42</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="4">
@@ -494,7 +494,7 @@
         <v>293.59</v>
       </c>
       <c r="D4" t="n">
-        <v>0.33</v>
+        <v>0.23</v>
       </c>
     </row>
     <row r="5">
@@ -508,7 +508,7 @@
         <v>289.53</v>
       </c>
       <c r="D5" t="n">
-        <v>0.24</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         <v>290.03</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="7">
@@ -536,7 +536,7 @@
         <v>287.65</v>
       </c>
       <c r="D7" t="n">
-        <v>0.22</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="8">
@@ -550,7 +550,7 @@
         <v>294.51</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>